<commit_message>
gui_single_)search.py uses NAV excel (pretend DB) to get RFID from Dock#, DockLine#,PackageLine# inputs
</commit_message>
<xml_diff>
--- a/A&B.xlsx
+++ b/A&B.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,10 +446,15 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>Unit ID</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>Pkg Line No</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>RFIDNumber</t>
         </is>
@@ -458,180 +463,190 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>S412354</t>
+          <t>S253441</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>4</v>
-      </c>
-      <c r="C2" t="n">
-        <v>7</v>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>E20047053E906026B1CC0105</t>
+        <v>1</v>
+      </c>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="n">
+        <v>3</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>E2004702ED6060268CB9010D</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>S452341</t>
+          <t>S243415</t>
         </is>
       </c>
       <c r="B3" t="n">
         <v>2</v>
       </c>
-      <c r="C3" t="n">
-        <v>1</v>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>E20047053EB06026B1CE010A</t>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="n">
+        <v>3</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>E2004704D9906026AB7C010D</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>S253441</t>
+          <t>S342451</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C4" t="n">
-        <v>3</v>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>E2004702ED6060268CB9010D</t>
+        <v>5</v>
+      </c>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="n">
+        <v>8</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>E2004704D9B06026AB7E0109</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>S542314</t>
+          <t>S452341</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>3</v>
-      </c>
-      <c r="C5" t="n">
+        <v>2</v>
+      </c>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="n">
         <v>1</v>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>E2004704D9A06026AB7D010E</t>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>E20047053EB06026B1CE010A</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>S234145</t>
+          <t>S412354</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1</v>
-      </c>
-      <c r="C6" t="n">
-        <v>8</v>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>E20047053EC06026B1CF0108</t>
+        <v>4</v>
+      </c>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="n">
+        <v>7</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>E20047053E906026B1CC0105</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>S534241</t>
+          <t>S234145</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>5</v>
-      </c>
-      <c r="C7" t="n">
-        <v>5</v>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>E20047053EA06026B1CD010A</t>
+        <v>1</v>
+      </c>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="n">
+        <v>8</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>E20047053EC06026B1CF0108</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t xml:space="preserve">S253441 </t>
+          <t>S534241</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1</v>
-      </c>
-      <c r="C8" t="n">
-        <v>2</v>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>E2004703EC9060269CAC0110</t>
+        <v>5</v>
+      </c>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="n">
+        <v>5</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>E20047053EA06026B1CD010A</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>S243415</t>
+          <t>S253441</t>
         </is>
       </c>
       <c r="B9" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" t="inlineStr"/>
+      <c r="D9" t="n">
         <v>2</v>
       </c>
-      <c r="C9" t="n">
-        <v>3</v>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>E2004704D9906026AB7C010D</t>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>E2004703EC9060269CAC0110</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>S342451</t>
+          <t>S454132</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>5</v>
-      </c>
-      <c r="C10" t="n">
-        <v>8</v>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>E2004704D9B06026AB7E0109</t>
+        <v>7</v>
+      </c>
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" t="n">
+        <v>3</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>E2004704D9C06026AB7F0114</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>S454132</t>
+          <t>S542314</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>7</v>
-      </c>
-      <c r="C11" t="n">
         <v>3</v>
       </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>E2004704D9C06026AB7F0114</t>
+      <c r="C11" t="inlineStr"/>
+      <c r="D11" t="n">
+        <v>1</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>E2004704D9A06026AB7D010E</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
success in 3 input - location found process
</commit_message>
<xml_diff>
--- a/A&B.xlsx
+++ b/A&B.xlsx
@@ -471,22 +471,22 @@
       </c>
       <c r="C2" t="inlineStr"/>
       <c r="D2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>E2004702ED6060268CB9010D</t>
+          <t>E2004703EC9060269CAC0110</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>S243415</t>
+          <t>S253441</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="n">
@@ -494,18 +494,18 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>E2004704D9906026AB7C010D</t>
+          <t>E2004702ED6060268CB9010D</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>S342451</t>
+          <t>S234145</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="n">
@@ -513,71 +513,71 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>E2004704D9B06026AB7E0109</t>
+          <t>E20047053EC06026B1CF0108</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>S452341</t>
+          <t>S454132</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>E20047053EB06026B1CE010A</t>
+          <t>E2004704D9C06026AB7F0114</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>S412354</t>
+          <t>S534241</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>E20047053E906026B1CC0105</t>
+          <t>E20047053EA06026B1CD010A</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>S234145</t>
+          <t>S243415</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>E20047053EC06026B1CF0108</t>
+          <t>E2004704D9906026AB7C010D</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>S534241</t>
+          <t>S342451</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -585,68 +585,68 @@
       </c>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>E20047053EA06026B1CD010A</t>
+          <t>E2004704D9B06026AB7E0109</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>S253441</t>
+          <t>S542314</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>E2004703EC9060269CAC0110</t>
+          <t>E2004704D9A06026AB7D010E</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>S454132</t>
+          <t>S452341</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>E2004704D9C06026AB7F0114</t>
+          <t>E20047053EB06026B1CE010A</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>S542314</t>
+          <t>S412354</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>E2004704D9A06026AB7D010E</t>
+          <t>E20047053E906026B1CC0105</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
updated NAV mock DB working
</commit_message>
<xml_diff>
--- a/A&B.xlsx
+++ b/A&B.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\krith\huskiesInvent\HuskiesInventTeam5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6CF94E1-692D-4D62-AD7E-9F38CEEAAD89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A808930-2CEB-483E-BC02-4F2A8125FB9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="50" windowWidth="16950" windowHeight="10480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,46 +20,31 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>RFIDNumber</t>
   </si>
   <si>
-    <t>E2004703EC9060269CAC0110</t>
-  </si>
-  <si>
-    <t>E2004702ED6060268CB9010D</t>
-  </si>
-  <si>
-    <t>E20047053EC06026B1CF0108</t>
-  </si>
-  <si>
-    <t>E2004704D9C06026AB7F0114</t>
-  </si>
-  <si>
-    <t>E20047053EA06026B1CD010A</t>
-  </si>
-  <si>
-    <t>E2004704D9906026AB7C010D</t>
-  </si>
-  <si>
-    <t>E2004704D9B06026AB7E0109</t>
-  </si>
-  <si>
-    <t>E2004704D9A06026AB7D010E</t>
-  </si>
-  <si>
-    <t>E20047053EB06026B1CE010A</t>
-  </si>
-  <si>
     <t>E20047053E906026B1CC0105</t>
+  </si>
+  <si>
+    <t>E2004703ECB060269CAE010F</t>
+  </si>
+  <si>
+    <t>E2004706F2306026CD06010D</t>
+  </si>
+  <si>
+    <t>E20047034BB06026929E010B</t>
+  </si>
+  <si>
+    <t>E200470496706026A74A0110</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -71,6 +56,11 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Inherit"/>
     </font>
   </fonts>
   <fills count="2">
@@ -108,10 +98,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -415,68 +408,49 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A11"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="A1:D11"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="26.90625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+    <row r="2" spans="1:1">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>10</v>
-      </c>
+    <row r="7" spans="1:1">
+      <c r="A7" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>